<commit_message>
added file checking functions
</commit_message>
<xml_diff>
--- a/inst/extdata/output_list.xlsx
+++ b/inst/extdata/output_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ccarmour.stu\Documents\GitHub\PEMprepr\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{773D4001-022D-44A4-9ABA-93E2C0B18B54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D9D8C42-72D5-48AE-A3DC-DE3DE549F029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{E31BD25C-5564-45B9-89E1-2A17F9A3385E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>description</t>
   </si>
@@ -57,16 +57,55 @@
     <t>AOI after being snapped to the nearest 100m extent.</t>
   </si>
   <si>
-    <t>var.name</t>
-  </si>
-  <si>
-    <t>obj.name</t>
-  </si>
-  <si>
     <t>AOI_original.gpkg</t>
   </si>
   <si>
     <t>AOI_snapped.gpkg</t>
+  </si>
+  <si>
+    <t>write.driver</t>
+  </si>
+  <si>
+    <t>st_read()</t>
+  </si>
+  <si>
+    <t>read.driver</t>
+  </si>
+  <si>
+    <t>st_write()</t>
+  </si>
+  <si>
+    <t>creator.func</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>dir_1010_vector</t>
+  </si>
+  <si>
+    <t>aoi.r.template</t>
+  </si>
+  <si>
+    <t>AOI_template_*m.tif</t>
+  </si>
+  <si>
+    <t>create_template()</t>
+  </si>
+  <si>
+    <t>rast()</t>
+  </si>
+  <si>
+    <t>writeRaster()</t>
+  </si>
+  <si>
+    <t>s.name</t>
+  </si>
+  <si>
+    <t>l.name</t>
+  </si>
+  <si>
+    <t>aoi_snap2()</t>
   </si>
 </sst>
 </file>
@@ -122,13 +161,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B1BD5729-CD4B-4D39-825E-4B2D51F57FF2}" name="Table1" displayName="Table1" ref="A1:D3" totalsRowShown="0">
-  <autoFilter ref="A1:D3" xr:uid="{B1BD5729-CD4B-4D39-825E-4B2D51F57FF2}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{40A9029A-022B-44DB-9E87-514C37007A81}" name="var.name"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B1BD5729-CD4B-4D39-825E-4B2D51F57FF2}" name="Table1" displayName="Table1" ref="A1:G4" totalsRowShown="0">
+  <autoFilter ref="A1:G4" xr:uid="{B1BD5729-CD4B-4D39-825E-4B2D51F57FF2}"/>
+  <tableColumns count="7">
     <tableColumn id="2" xr3:uid="{22A413C4-B8F3-44A6-A170-E76FE867910D}" name="description"/>
+    <tableColumn id="1" xr3:uid="{40A9029A-022B-44DB-9E87-514C37007A81}" name="s.name"/>
     <tableColumn id="3" xr3:uid="{82424074-AE09-4F69-9FE3-AA261808521A}" name="f.ids.path"/>
-    <tableColumn id="4" xr3:uid="{ECBFBA0D-CE93-4508-8A97-115888C41D1B}" name="obj.name"/>
+    <tableColumn id="4" xr3:uid="{ECBFBA0D-CE93-4508-8A97-115888C41D1B}" name="l.name"/>
+    <tableColumn id="7" xr3:uid="{9E46435A-414E-47F3-9CB7-495950DF3C81}" name="creator.func"/>
+    <tableColumn id="5" xr3:uid="{0589D967-E9A1-4B73-9721-D05064CBEB26}" name="read.driver"/>
+    <tableColumn id="6" xr3:uid="{F1508FFA-3862-40AE-A7C0-93D21FD62B17}" name="write.driver"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -431,60 +473,109 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAD51235-5DFA-4F6A-8756-158593A3D011}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="49.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="49.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="5" max="6" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
         <v>10</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>